<commit_message>
update database, renamed one cateogry
</commit_message>
<xml_diff>
--- a/example_base.xlsx
+++ b/example_base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1de75ab757d4e5e4/Pulpit/studia/swd/projekt/Trip-selection-support-system/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\SEM_5_SWD\koncowy projekt\Trip-selection-support-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{067FD9B5-9A6A-4DED-AC52-B537685AD645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CBF99A3-0BBA-4867-A38D-339A82862D5A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68110EE2-145A-4EBF-8877-5BAEF5EE5F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{82038EAF-E625-447E-8475-976217D15C54}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{82038EAF-E625-447E-8475-976217D15C54}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Miasto</t>
   </si>
   <si>
-    <t>Minimalny czas podróży (min)</t>
-  </si>
-  <si>
     <t>Cena za dobę za osobę (PLN)</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Zabytki i kultura</t>
   </si>
   <si>
-    <t>Parki Narodowe</t>
-  </si>
-  <si>
     <t>Nowy Jork</t>
   </si>
   <si>
@@ -603,6 +597,12 @@
   </si>
   <si>
     <t>Malta</t>
+  </si>
+  <si>
+    <t>Maksymalny czas podróży (min)</t>
+  </si>
+  <si>
+    <t>Natura i Parki Narodowe</t>
   </si>
 </sst>
 </file>
@@ -995,68 +995,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D82785-369F-4861-81B1-363C2DA20361}">
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P106" sqref="P106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1100,7 +1101,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1320,7 +1321,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1584,7 +1585,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1760,7 +1761,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1892,7 +1893,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2068,7 +2069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2112,7 +2113,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2288,7 +2289,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2508,7 +2509,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2596,7 +2597,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2684,7 +2685,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2728,7 +2729,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2772,7 +2773,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2816,7 +2817,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2860,7 +2861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2904,7 +2905,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2948,7 +2949,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3036,7 +3037,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3124,7 +3125,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3212,7 +3213,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3256,7 +3257,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3300,7 +3301,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3388,7 +3389,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3476,7 +3477,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3520,7 +3521,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3564,7 +3565,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3608,7 +3609,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3696,7 +3697,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3740,7 +3741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3784,7 +3785,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3828,7 +3829,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3872,7 +3873,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3916,7 +3917,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3960,7 +3961,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4004,7 +4005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4048,7 +4049,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4092,7 +4093,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4136,7 +4137,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4180,7 +4181,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4224,7 +4225,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4268,7 +4269,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4312,7 +4313,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4356,7 +4357,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4400,7 +4401,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4488,7 +4489,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4576,7 +4577,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -4620,7 +4621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -4664,7 +4665,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -4708,7 +4709,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4796,7 +4797,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -4840,7 +4841,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4884,7 +4885,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4928,7 +4929,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4972,7 +4973,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -5016,7 +5017,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -5060,7 +5061,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -5104,7 +5105,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -5148,7 +5149,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -5192,7 +5193,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -5236,7 +5237,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -5280,7 +5281,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -5324,7 +5325,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -5368,7 +5369,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -5412,7 +5413,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -5456,7 +5457,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -5510,1137 +5511,1137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2AA7CC-E4F4-4113-952C-715A94BCEB78}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C59" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C62" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C64" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C65" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C70" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C72" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C75" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C77" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C78" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C80" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C81" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C82" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C83" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C84" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C86" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C87" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C88" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C89" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C90" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C91" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C92" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C93" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C94" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C95" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C96" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C97" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C98" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C99" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C100" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C101" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C102" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>